<commit_message>
Dynamic code added to Pattern
</commit_message>
<xml_diff>
--- a/testData/gmail.xlsx
+++ b/testData/gmail.xlsx
@@ -14,15 +14,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Critical security alert</t>
+    <t>Test Mail</t>
   </si>
   <si>
-    <t>Sign-in attempt was blocked
-mailfortesting086@gmail.com
-Someone just used your password to try to sign in to your account. Google blocked them, but you should check what happened.
-Check activity
-You received this email to let you know about important changes to your Google Account and services.
-© 2020 Google LLC, 1600 Amphitheatre Parkway, Mountain View, CA 94043, USA</t>
+    <t>Hello Manas</t>
   </si>
 </sst>
 </file>

</xml_diff>